<commit_message>
W LogsTotal , LogsProfile  update
</commit_message>
<xml_diff>
--- a/public/images/uploads/import_file.xlsx
+++ b/public/images/uploads/import_file.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>ซื้อ</t>
   </si>
@@ -75,43 +75,16 @@
     <t>at_pay</t>
   </si>
   <si>
-    <t>TMB</t>
-  </si>
-  <si>
     <t>ขาย</t>
   </si>
   <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>PTT</t>
-  </si>
-  <si>
-    <t>SIRI</t>
-  </si>
-  <si>
     <t>BLS</t>
   </si>
   <si>
     <t>KTB</t>
   </si>
   <si>
-    <t>LH</t>
-  </si>
-  <si>
-    <t>DTAC</t>
-  </si>
-  <si>
     <t>EFORL</t>
-  </si>
-  <si>
-    <t>BMCL</t>
-  </si>
-  <si>
-    <t>KBANK</t>
-  </si>
-  <si>
-    <t>INTUCH</t>
   </si>
   <si>
     <t>VGI</t>
@@ -635,7 +608,7 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,34 +660,34 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>845</v>
+        <v>865</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
-        <v>4</v>
+        <v>200</v>
       </c>
       <c r="E2" s="1">
-        <v>63.25</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="F2" s="1">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="G2" s="1">
-        <v>0.43</v>
+        <v>0.37</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>253.43</v>
+        <v>223.63</v>
       </c>
       <c r="J2" s="3">
-        <v>42263</v>
+        <v>42268</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>2</v>
@@ -723,46 +696,46 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>846</v>
+        <v>866</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1">
-        <v>75.75</v>
-      </c>
-      <c r="F3" s="1">
-        <v>757.5</v>
+        <v>17.8</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1780</v>
       </c>
       <c r="G3" s="1">
-        <v>1.28</v>
+        <v>0.34</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="1">
-        <v>758.78</v>
+      <c r="I3" s="9">
+        <v>1783.01</v>
       </c>
       <c r="J3" s="3">
-        <v>42263</v>
+        <v>42268</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>847</v>
+        <v>867</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -771,638 +744,264 @@
         <v>100</v>
       </c>
       <c r="E4" s="1">
-        <v>1.67</v>
+        <v>3.72</v>
       </c>
       <c r="F4" s="1">
-        <v>167</v>
+        <v>372</v>
       </c>
       <c r="G4" s="1">
-        <v>0.28000000000000003</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>166.72</v>
+        <v>371.37</v>
       </c>
       <c r="J4" s="3">
-        <v>42263</v>
+        <v>42268</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>848</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1">
-        <v>100</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.66</v>
-      </c>
-      <c r="F5" s="1">
-        <v>166</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>165.72</v>
-      </c>
-      <c r="J5" s="3">
-        <v>42263</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>849</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1">
-        <v>100</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2.46</v>
-      </c>
-      <c r="F6" s="1">
-        <v>246</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>245.58</v>
-      </c>
-      <c r="J6" s="3">
-        <v>42263</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>850</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1">
-        <v>100</v>
-      </c>
-      <c r="E7" s="1">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="F7" s="9">
-        <v>1790</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <v>1793.04</v>
-      </c>
-      <c r="J7" s="3">
-        <v>42263</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>851</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1">
-        <v>100</v>
-      </c>
-      <c r="E8" s="1">
-        <v>7.95</v>
-      </c>
-      <c r="F8" s="1">
-        <v>795</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>793.66</v>
-      </c>
-      <c r="J8" s="3">
-        <v>42263</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>852</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>200</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.79</v>
-      </c>
-      <c r="F9" s="1">
-        <v>158</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.27</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>158.27000000000001</v>
-      </c>
-      <c r="J9" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>853</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1">
-        <v>100</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1.78</v>
-      </c>
-      <c r="F10" s="1">
-        <v>178</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>178.3</v>
-      </c>
-      <c r="J10" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>854</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="1">
-        <v>200</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.91</v>
-      </c>
-      <c r="F11" s="1">
-        <v>182</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.31</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>182.31</v>
-      </c>
-      <c r="J11" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>855</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <v>500</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1.05</v>
-      </c>
-      <c r="F12" s="1">
-        <v>525</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>524.11</v>
-      </c>
-      <c r="J12" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>856</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="1">
-        <v>500</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.05</v>
-      </c>
-      <c r="F13" s="1">
-        <v>525</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>524.11</v>
-      </c>
-      <c r="J13" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>857</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>255</v>
-      </c>
-      <c r="F14" s="1">
-        <v>255</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>254.57</v>
-      </c>
-      <c r="J14" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>858</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1">
-        <v>179</v>
-      </c>
-      <c r="F15" s="1">
-        <v>895</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.17</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>896.51</v>
-      </c>
-      <c r="J15" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>859</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5</v>
-      </c>
-      <c r="E16" s="1">
-        <v>180.5</v>
-      </c>
-      <c r="F16" s="1">
-        <v>902.5</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.17</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>900.98</v>
-      </c>
-      <c r="J16" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>860</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100</v>
-      </c>
-      <c r="E17" s="1">
-        <v>18.2</v>
-      </c>
-      <c r="F17" s="9">
-        <v>1820</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
-        <v>1816.91</v>
-      </c>
-      <c r="J17" s="3">
-        <v>42264</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>861</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="1">
-        <v>100</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1.65</v>
-      </c>
-      <c r="F18" s="1">
-        <v>165</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>165.28</v>
-      </c>
-      <c r="J18" s="3">
-        <v>42267</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>862</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1">
-        <v>100</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2.52</v>
-      </c>
-      <c r="F19" s="1">
-        <v>252</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>251.57</v>
-      </c>
-      <c r="J19" s="3">
-        <v>42267</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>863</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="1">
-        <v>100</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3.66</v>
-      </c>
-      <c r="F20" s="1">
-        <v>366</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>366.61</v>
-      </c>
-      <c r="J20" s="3">
-        <v>42267</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>864</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="1">
-        <v>100</v>
-      </c>
-      <c r="E21" s="1">
-        <v>8.25</v>
-      </c>
-      <c r="F21" s="1">
-        <v>825</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>823.6</v>
-      </c>
-      <c r="J21" s="3">
-        <v>42267</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
W LogsProfile dynamic update
</commit_message>
<xml_diff>
--- a/public/images/uploads/import_file.xlsx
+++ b/public/images/uploads/import_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momo\Desktop\_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
   <si>
     <t>ซื้อ</t>
   </si>
@@ -87,31 +87,34 @@
     <t>ขาย</t>
   </si>
   <si>
-    <t>KTB</t>
-  </si>
-  <si>
     <t>due_date</t>
   </si>
   <si>
+    <t>DTAC</t>
+  </si>
+  <si>
+    <t>DTAC01P1512A</t>
+  </si>
+  <si>
+    <t>S5001C1512A</t>
+  </si>
+  <si>
+    <t>INTUCH</t>
+  </si>
+  <si>
+    <t>S5001P1511B</t>
+  </si>
+  <si>
+    <t>LHK</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
     <t>ADVANC</t>
   </si>
   <si>
-    <t>INTUCH</t>
-  </si>
-  <si>
-    <t>BLAND</t>
-  </si>
-  <si>
-    <t>DTAC</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>S5001C1511B</t>
-  </si>
-  <si>
-    <t>LH</t>
+    <t>TMB</t>
   </si>
 </sst>
 </file>
@@ -635,7 +638,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,92 +689,96 @@
         <v>14</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>935</v>
+        <v>952</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="E2" s="1">
-        <v>220</v>
+        <v>0.74</v>
       </c>
       <c r="F2" s="1">
-        <v>220</v>
+        <v>370</v>
       </c>
       <c r="G2" s="1">
-        <v>0.37</v>
+        <v>0.62</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>220.37</v>
+        <v>370.62</v>
       </c>
       <c r="J2" s="3">
-        <v>42282</v>
+        <v>42284</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="M2" s="3">
         <f>J2</f>
-        <v>42282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>936</v>
+        <v>953</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="E3" s="1">
-        <v>71.75</v>
-      </c>
-      <c r="F3" s="1">
-        <v>717.5</v>
+        <v>3.02</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1208</v>
       </c>
       <c r="G3" s="1">
-        <v>1.21</v>
+        <v>2.04</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="1">
-        <v>718.71</v>
+      <c r="I3" s="9">
+        <v>1205.96</v>
       </c>
       <c r="J3" s="3">
-        <v>42282</v>
+        <v>42284</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="M3" s="3">
         <f t="shared" ref="M3:M42" si="0">J3</f>
-        <v>42282</v>
+        <v>42284</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>937</v>
+        <v>954</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -780,25 +787,25 @@
         <v>24</v>
       </c>
       <c r="D4" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>1.47</v>
-      </c>
-      <c r="F4" s="9">
-        <v>735</v>
+        <v>73.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>367.5</v>
       </c>
       <c r="G4" s="1">
-        <v>1.24</v>
+        <v>0.62</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="9">
-        <v>733.76</v>
+      <c r="I4" s="1">
+        <v>366.88</v>
       </c>
       <c r="J4" s="3">
-        <v>42282</v>
+        <v>42284</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>2</v>
@@ -806,12 +813,12 @@
       <c r="L4" s="4"/>
       <c r="M4" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>938</v>
+        <v>955</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -820,427 +827,521 @@
         <v>25</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1">
-        <v>55.25</v>
-      </c>
-      <c r="F5" s="9">
-        <v>552.5</v>
+        <v>0.7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>70</v>
       </c>
       <c r="G5" s="1">
-        <v>0.93</v>
+        <v>0.12</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="9">
-        <v>551.57000000000005</v>
+      <c r="I5" s="1">
+        <v>69.88</v>
       </c>
       <c r="J5" s="3">
-        <v>42282</v>
+        <v>42284</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
+        <v>42284</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>939</v>
+        <v>956</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="1">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1">
-        <v>0.91</v>
+        <v>2.98</v>
       </c>
       <c r="F6" s="1">
-        <v>455</v>
+        <v>298</v>
       </c>
       <c r="G6" s="1">
-        <v>0.77</v>
+        <v>0.06</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>454.23</v>
+        <v>298.5</v>
       </c>
       <c r="J6" s="3">
-        <v>42282</v>
+        <v>42284</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
+        <v>42284</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>940</v>
+        <v>957</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E7" s="1">
-        <v>250</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F7" s="1">
-        <v>250</v>
+        <v>805</v>
       </c>
       <c r="G7" s="1">
-        <v>0.42</v>
+        <v>0.15</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>249.58</v>
+        <v>803.64</v>
       </c>
       <c r="J7" s="3">
-        <v>42282</v>
+        <v>42284</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
+        <v>42284</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>941</v>
+        <v>958</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
         <v>200</v>
       </c>
       <c r="E8" s="1">
-        <v>1.1299999999999999</v>
+        <v>0.66</v>
       </c>
       <c r="F8" s="1">
-        <v>226</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1">
-        <v>0.38</v>
+        <v>0.22</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>225.62</v>
+        <v>132.22</v>
       </c>
       <c r="J8" s="3">
-        <v>42282</v>
+        <v>42285</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="4" t="b">
+      <c r="L8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>942</v>
+        <v>959</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="F9" s="1">
-        <v>860</v>
+        <v>234</v>
       </c>
       <c r="G9" s="1">
-        <v>0.17</v>
+        <v>0.4</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>861.46</v>
+        <v>233.6</v>
       </c>
       <c r="J9" s="3">
-        <v>42282</v>
+        <v>42285</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="4"/>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>943</v>
+        <v>960</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
-        <v>172</v>
+        <v>57.25</v>
       </c>
       <c r="F10" s="1">
-        <v>688</v>
+        <v>515.25</v>
       </c>
       <c r="G10" s="1">
-        <v>0.12</v>
+        <v>0.87</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>689.16</v>
+        <v>514.38</v>
       </c>
       <c r="J10" s="3">
-        <v>42282</v>
+        <v>42285</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="L10" s="4"/>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="F11" s="1">
-        <v>800</v>
+        <v>269</v>
       </c>
       <c r="G11" s="1">
-        <v>0.17</v>
+        <v>0.45</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <v>801.35</v>
+        <v>268.55</v>
       </c>
       <c r="J11" s="3">
-        <v>42282</v>
+        <v>42285</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>945</v>
+        <v>962</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="E12" s="1">
-        <v>17.100000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="F12" s="1">
-        <v>171</v>
+        <v>375</v>
       </c>
       <c r="G12" s="1">
-        <v>0.03</v>
+        <v>0.63</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>170.71</v>
+        <v>374.37</v>
       </c>
       <c r="J12" s="3">
-        <v>42282</v>
+        <v>42285</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="L12" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>42282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>946</v>
+        <v>963</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="F13" s="1">
+        <v>130</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>129.78</v>
+      </c>
+      <c r="J13" s="3">
+        <v>42285</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>42285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>964</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1">
+        <v>200</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2.54</v>
+      </c>
+      <c r="F14" s="1">
+        <v>508</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>507.14</v>
+      </c>
+      <c r="J14" s="3">
+        <v>42285</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>42285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>965</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="1">
-        <v>100</v>
-      </c>
-      <c r="E13" s="1">
-        <v>172.5</v>
-      </c>
-      <c r="F13" s="9">
-        <v>17250</v>
-      </c>
-      <c r="G13" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>17220.87</v>
-      </c>
-      <c r="J13" s="3">
-        <v>42282</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <v>177</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1416</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1418.39</v>
+      </c>
+      <c r="J15" s="3">
+        <v>42285</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="3">
-        <f t="shared" si="0"/>
-        <v>42282</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
       <c r="L15" s="4"/>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="2"/>
+      <c r="A16" s="1">
+        <v>966</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1">
+        <v>100</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>810</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>811.37</v>
+      </c>
+      <c r="J16" s="3">
+        <v>42285</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L16" s="4"/>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="A17" s="1">
+        <v>967</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8.25</v>
+      </c>
+      <c r="F17" s="1">
+        <v>825</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>823.6</v>
+      </c>
+      <c r="J17" s="3">
+        <v>42285</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="4"/>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>